<commit_message>
Update planning file and adding status update
</commit_message>
<xml_diff>
--- a/Planning Sheet.xlsx
+++ b/Planning Sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\capgemini\Capgemini_ADAPT\Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18F98FFE-362A-4A93-B31F-B3BB0E02B693}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E714F6B-094A-40B9-AD36-010C50E26B7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{5D0DB168-4E03-4E20-AA99-CAAE4AA3C970}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="26">
   <si>
     <t>Task no.</t>
   </si>
@@ -96,26 +96,26 @@
     <t>STATEMENTS</t>
   </si>
   <si>
-    <t>Navbar and display picture done .Working on flight details</t>
+    <t>Completed</t>
+  </si>
+  <si>
+    <t>Merging and connected to home page foem left</t>
+  </si>
+  <si>
+    <t>Database Connection left</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF222222"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
@@ -130,7 +130,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -161,6 +161,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="5">
     <border>
@@ -226,46 +232,70 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="1" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="1" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="1" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="2" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="2" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="2" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="2" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="1" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="1" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="1" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="1" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -581,384 +611,411 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BFB52314-F248-404A-A220-498A93624F9C}">
-  <dimension ref="A1:J15"/>
+  <dimension ref="A1:J13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+      <selection activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="15.33203125" customWidth="1"/>
     <col min="3" max="3" width="21.21875" customWidth="1"/>
+    <col min="8" max="8" width="18.21875" customWidth="1"/>
     <col min="10" max="10" width="77.21875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2" t="s">
+      <c r="B1" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="J1" s="15" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="3">
-        <v>1</v>
-      </c>
-      <c r="B2" s="4" t="s">
+      <c r="A2" s="9">
+        <v>4</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="13">
+        <v>2</v>
+      </c>
+      <c r="F2" s="14">
+        <v>45068</v>
+      </c>
+      <c r="G2" s="14">
+        <v>45069</v>
+      </c>
+      <c r="H2" s="14">
+        <v>45069</v>
+      </c>
+      <c r="I2" s="19">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C3" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="5">
-        <v>1</v>
-      </c>
-      <c r="F2" s="6">
+      <c r="E3" s="3">
+        <v>1</v>
+      </c>
+      <c r="F3" s="4">
         <v>45069</v>
       </c>
-      <c r="G2" s="6">
+      <c r="G3" s="4">
         <v>45069</v>
       </c>
-      <c r="H2" s="6">
+      <c r="H3" s="4">
         <v>45069</v>
       </c>
-      <c r="I2" s="7"/>
-      <c r="J2" s="11"/>
-    </row>
-    <row r="3" spans="1:10" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="3">
+      <c r="I3" s="6">
+        <v>1</v>
+      </c>
+      <c r="J3" s="7" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="1">
+        <v>3</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" s="3">
+        <v>1</v>
+      </c>
+      <c r="F4" s="4">
+        <v>45069</v>
+      </c>
+      <c r="G4" s="4">
+        <v>45071</v>
+      </c>
+      <c r="H4" s="4">
+        <v>45071</v>
+      </c>
+      <c r="I4" s="18">
+        <v>0.9</v>
+      </c>
+      <c r="J4" s="8" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="1">
+        <v>8</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E5" s="3">
+        <v>1</v>
+      </c>
+      <c r="F5" s="4">
+        <v>45069</v>
+      </c>
+      <c r="G5" s="4">
+        <v>45070</v>
+      </c>
+      <c r="H5" s="4">
+        <v>45070</v>
+      </c>
+      <c r="I5" s="5">
+        <v>1</v>
+      </c>
+      <c r="J5" s="21" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="1">
+        <v>10</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E6" s="3">
+        <v>1</v>
+      </c>
+      <c r="F6" s="4">
+        <v>45069</v>
+      </c>
+      <c r="G6" s="4">
+        <v>45069</v>
+      </c>
+      <c r="H6" s="4">
+        <v>45069</v>
+      </c>
+      <c r="I6" s="6">
+        <v>1</v>
+      </c>
+      <c r="J6" s="20" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="1">
+        <v>5</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E7" s="3">
+        <v>1</v>
+      </c>
+      <c r="F7" s="4">
+        <v>45070</v>
+      </c>
+      <c r="G7" s="4">
+        <v>45070</v>
+      </c>
+      <c r="H7" s="17">
+        <v>45071</v>
+      </c>
+      <c r="I7" s="18">
+        <v>0.9</v>
+      </c>
+      <c r="J7" s="16" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="1">
         <v>2</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B8" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C8" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D8" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="5">
-        <v>1</v>
-      </c>
-      <c r="F3" s="6">
+      <c r="E8" s="3">
+        <v>1</v>
+      </c>
+      <c r="F8" s="4">
         <v>45071</v>
       </c>
-      <c r="G3" s="6">
+      <c r="G8" s="4">
         <v>45071</v>
       </c>
-      <c r="H3" s="4"/>
-      <c r="I3" s="4"/>
-      <c r="J3" s="13"/>
-    </row>
-    <row r="4" spans="1:10" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="3">
-        <v>3</v>
-      </c>
-      <c r="B4" s="4" t="s">
+      <c r="H8" s="17">
+        <v>45071</v>
+      </c>
+      <c r="I8" s="6">
+        <v>1</v>
+      </c>
+      <c r="J8" s="8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="1">
+        <v>7</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E9" s="3">
+        <v>1</v>
+      </c>
+      <c r="F9" s="4">
+        <v>45071</v>
+      </c>
+      <c r="G9" s="4">
+        <v>45072</v>
+      </c>
+      <c r="H9" s="2"/>
+      <c r="I9" s="2"/>
+      <c r="J9" s="2"/>
+    </row>
+    <row r="10" spans="1:10" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="1">
+        <v>11</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E10" s="3">
+        <v>1</v>
+      </c>
+      <c r="F10" s="4">
+        <v>45071</v>
+      </c>
+      <c r="G10" s="4">
+        <v>45072</v>
+      </c>
+      <c r="H10" s="2"/>
+      <c r="I10" s="2"/>
+      <c r="J10" s="2"/>
+    </row>
+    <row r="11" spans="1:10" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="1">
         <v>12</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="B11" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E11" s="3">
+        <v>1</v>
+      </c>
+      <c r="F11" s="4">
+        <v>45071</v>
+      </c>
+      <c r="G11" s="4">
+        <v>45071</v>
+      </c>
+      <c r="H11" s="17">
+        <v>45071</v>
+      </c>
+      <c r="I11" s="18">
+        <v>0.9</v>
+      </c>
+      <c r="J11" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="1">
+        <v>6</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E12" s="3">
+        <v>1</v>
+      </c>
+      <c r="F12" s="4">
+        <v>45072</v>
+      </c>
+      <c r="G12" s="4">
+        <v>45075</v>
+      </c>
+      <c r="H12" s="2"/>
+      <c r="I12" s="2"/>
+      <c r="J12" s="2"/>
+    </row>
+    <row r="13" spans="1:10" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="1">
         <v>9</v>
       </c>
-      <c r="D4" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E4" s="5">
-        <v>1</v>
-      </c>
-      <c r="F4" s="6">
-        <v>45069</v>
-      </c>
-      <c r="G4" s="6">
-        <v>45071</v>
-      </c>
-      <c r="H4" s="4"/>
-      <c r="I4" s="7"/>
-      <c r="J4" s="13"/>
-    </row>
-    <row r="5" spans="1:10" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="3">
-        <v>4</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C5" s="4" t="s">
+      <c r="B13" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C13" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D5" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E5" s="5">
-        <v>2</v>
-      </c>
-      <c r="F5" s="6">
-        <v>45068</v>
-      </c>
-      <c r="G5" s="6">
-        <v>45069</v>
-      </c>
-      <c r="H5" s="6">
-        <v>45069</v>
-      </c>
-      <c r="I5" s="8">
-        <v>0.7</v>
-      </c>
-      <c r="J5" s="12"/>
-    </row>
-    <row r="6" spans="1:10" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="3">
-        <v>5</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E6" s="5">
-        <v>1</v>
-      </c>
-      <c r="F6" s="6">
-        <v>45070</v>
-      </c>
-      <c r="G6" s="6">
-        <v>45070</v>
-      </c>
-      <c r="H6" s="4"/>
-      <c r="I6" s="4"/>
-      <c r="J6" s="4"/>
-    </row>
-    <row r="7" spans="1:10" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="3">
-        <v>6</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E7" s="5">
-        <v>1</v>
-      </c>
-      <c r="F7" s="6">
-        <v>45072</v>
-      </c>
-      <c r="G7" s="6">
-        <v>45075</v>
-      </c>
-      <c r="H7" s="4"/>
-      <c r="I7" s="4"/>
-      <c r="J7" s="4"/>
-    </row>
-    <row r="8" spans="1:10" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="3">
-        <v>7</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D8" s="4" t="s">
+      <c r="D13" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="E8" s="5">
-        <v>1</v>
-      </c>
-      <c r="F8" s="6">
-        <v>45071</v>
-      </c>
-      <c r="G8" s="6">
-        <v>45072</v>
-      </c>
-      <c r="H8" s="4"/>
-      <c r="I8" s="4"/>
-      <c r="J8" s="4"/>
-    </row>
-    <row r="9" spans="1:10" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="3">
-        <v>8</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="E9" s="5">
-        <v>1</v>
-      </c>
-      <c r="F9" s="6">
-        <v>45069</v>
-      </c>
-      <c r="G9" s="6">
-        <v>45070</v>
-      </c>
-      <c r="H9" s="6">
-        <v>45070</v>
-      </c>
-      <c r="I9" s="8">
-        <v>0.8</v>
-      </c>
-      <c r="J9" s="12"/>
-    </row>
-    <row r="10" spans="1:10" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="3">
-        <v>9</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="E10" s="5">
-        <v>1</v>
-      </c>
-      <c r="F10" s="6">
+      <c r="E13" s="3">
+        <v>1</v>
+      </c>
+      <c r="F13" s="4">
         <v>45073</v>
       </c>
-      <c r="G10" s="6">
+      <c r="G13" s="4">
         <v>45074</v>
       </c>
-      <c r="H10" s="4"/>
-      <c r="I10" s="4"/>
-      <c r="J10" s="4"/>
-    </row>
-    <row r="11" spans="1:10" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="3">
-        <v>10</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E11" s="5">
-        <v>1</v>
-      </c>
-      <c r="F11" s="6">
-        <v>45069</v>
-      </c>
-      <c r="G11" s="6">
-        <v>45069</v>
-      </c>
-      <c r="H11" s="6">
-        <v>45069</v>
-      </c>
-      <c r="I11" s="10">
-        <v>0.8</v>
-      </c>
-      <c r="J11" s="13" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="3">
-        <v>11</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D12" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E12" s="5">
-        <v>1</v>
-      </c>
-      <c r="F12" s="6">
-        <v>45071</v>
-      </c>
-      <c r="G12" s="6">
-        <v>45072</v>
-      </c>
-      <c r="H12" s="4"/>
-      <c r="I12" s="4"/>
-      <c r="J12" s="4"/>
-    </row>
-    <row r="13" spans="1:10" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="3">
-        <v>12</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D13" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="E13" s="5">
-        <v>1</v>
-      </c>
-      <c r="F13" s="6">
-        <v>45071</v>
-      </c>
-      <c r="G13" s="6">
-        <v>45071</v>
-      </c>
-      <c r="H13" s="4"/>
-      <c r="I13" s="4"/>
-      <c r="J13" s="4"/>
-    </row>
-    <row r="14" spans="1:10" ht="15" x14ac:dyDescent="0.3">
-      <c r="A14" s="9"/>
-    </row>
-    <row r="15" spans="1:10" ht="15" x14ac:dyDescent="0.3">
-      <c r="A15" s="9"/>
+      <c r="H13" s="2"/>
+      <c r="I13" s="2"/>
+      <c r="J13" s="2"/>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1:J13">
+    <sortCondition ref="F2:F13"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
home page of flight booking system
</commit_message>
<xml_diff>
--- a/Planning Sheet.xlsx
+++ b/Planning Sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\capgemini\Capgemini_ADAPT\Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E714F6B-094A-40B9-AD36-010C50E26B7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A0E9096-027F-45C5-ABDF-CCC873C28886}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{5D0DB168-4E03-4E20-AA99-CAAE4AA3C970}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="26">
   <si>
     <t>Task no.</t>
   </si>
@@ -45,9 +45,6 @@
     <t>End date</t>
   </si>
   <si>
-    <t>Actual ETA</t>
-  </si>
-  <si>
     <t>STATUS</t>
   </si>
   <si>
@@ -93,16 +90,19 @@
     <t>home</t>
   </si>
   <si>
-    <t>STATEMENTS</t>
-  </si>
-  <si>
     <t>Completed</t>
   </si>
   <si>
-    <t>Merging and connected to home page foem left</t>
-  </si>
-  <si>
     <t>Database Connection left</t>
+  </si>
+  <si>
+    <t>Remarks/Comments</t>
+  </si>
+  <si>
+    <t>Login to Home connection database connectivity</t>
+  </si>
+  <si>
+    <t>Merging and connected to home page form left</t>
   </si>
 </sst>
 </file>
@@ -232,7 +232,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
@@ -281,9 +281,6 @@
     </xf>
     <xf numFmtId="9" fontId="1" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="1" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="1" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -611,10 +608,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BFB52314-F248-404A-A220-498A93624F9C}">
-  <dimension ref="A1:J13"/>
+  <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J20" sqref="J20"/>
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -622,10 +619,11 @@
     <col min="2" max="2" width="15.33203125" customWidth="1"/>
     <col min="3" max="3" width="21.21875" customWidth="1"/>
     <col min="8" max="8" width="18.21875" customWidth="1"/>
+    <col min="9" max="9" width="51.88671875" customWidth="1"/>
     <col min="10" max="10" width="77.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
@@ -648,25 +646,22 @@
       <c r="H1" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="J1" s="15" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I1" s="15" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="9">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B2" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="11" t="s">
-        <v>15</v>
-      </c>
       <c r="D2" s="11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E2" s="13">
         <v>2</v>
@@ -677,25 +672,25 @@
       <c r="G2" s="14">
         <v>45069</v>
       </c>
-      <c r="H2" s="14">
-        <v>45069</v>
-      </c>
-      <c r="I2" s="19">
+      <c r="H2" s="18">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="D3" s="2" t="s">
         <v>9</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>10</v>
       </c>
       <c r="E3" s="3">
         <v>1</v>
@@ -706,28 +701,25 @@
       <c r="G3" s="4">
         <v>45069</v>
       </c>
-      <c r="H3" s="4">
-        <v>45069</v>
-      </c>
-      <c r="I3" s="6">
-        <v>1</v>
-      </c>
-      <c r="J3" s="7" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H3" s="6">
+        <v>1</v>
+      </c>
+      <c r="I3" s="7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="2" t="s">
         <v>12</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>13</v>
       </c>
       <c r="E4" s="3">
         <v>1</v>
@@ -738,28 +730,25 @@
       <c r="G4" s="4">
         <v>45071</v>
       </c>
-      <c r="H4" s="4">
-        <v>45071</v>
-      </c>
-      <c r="I4" s="18">
+      <c r="H4" s="17">
         <v>0.9</v>
       </c>
-      <c r="J4" s="8" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I4" s="8" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
+        <v>4</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>9</v>
-      </c>
       <c r="D5" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E5" s="3">
         <v>1</v>
@@ -770,28 +759,25 @@
       <c r="G5" s="4">
         <v>45070</v>
       </c>
-      <c r="H5" s="4">
-        <v>45070</v>
-      </c>
-      <c r="I5" s="5">
-        <v>1</v>
-      </c>
-      <c r="J5" s="21" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H5" s="5">
+        <v>1</v>
+      </c>
+      <c r="I5" s="20" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E6" s="3">
         <v>1</v>
@@ -802,28 +788,25 @@
       <c r="G6" s="4">
         <v>45069</v>
       </c>
-      <c r="H6" s="4">
-        <v>45069</v>
-      </c>
-      <c r="I6" s="6">
-        <v>1</v>
-      </c>
-      <c r="J6" s="20" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H6" s="6">
+        <v>1</v>
+      </c>
+      <c r="I6" s="19" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E7" s="3">
         <v>1</v>
@@ -835,27 +818,22 @@
         <v>45070</v>
       </c>
       <c r="H7" s="17">
-        <v>45071</v>
-      </c>
-      <c r="I7" s="18">
         <v>0.9</v>
       </c>
-      <c r="J7" s="16" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I7" s="16"/>
+    </row>
+    <row r="8" spans="1:9" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="1">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C8" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8" s="2" t="s">
         <v>9</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>10</v>
       </c>
       <c r="E8" s="3">
         <v>1</v>
@@ -866,28 +844,25 @@
       <c r="G8" s="4">
         <v>45071</v>
       </c>
-      <c r="H8" s="17">
-        <v>45071</v>
-      </c>
-      <c r="I8" s="6">
-        <v>1</v>
-      </c>
-      <c r="J8" s="8" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H8" s="6">
+        <v>1</v>
+      </c>
+      <c r="I8" s="8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B9" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D9" s="2" t="s">
         <v>17</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>18</v>
       </c>
       <c r="E9" s="3">
         <v>1</v>
@@ -900,46 +875,44 @@
       </c>
       <c r="H9" s="2"/>
       <c r="I9" s="2"/>
-      <c r="J9" s="2"/>
-    </row>
-    <row r="10" spans="1:10" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="10" spans="1:9" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="1">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E10" s="3">
         <v>1</v>
       </c>
       <c r="F10" s="4">
-        <v>45071</v>
+        <v>45072</v>
       </c>
       <c r="G10" s="4">
-        <v>45072</v>
+        <v>45073</v>
       </c>
       <c r="H10" s="2"/>
       <c r="I10" s="2"/>
-      <c r="J10" s="2"/>
-    </row>
-    <row r="11" spans="1:10" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="11" spans="1:9" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="1">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E11" s="3">
         <v>1</v>
@@ -951,53 +924,49 @@
         <v>45071</v>
       </c>
       <c r="H11" s="17">
-        <v>45071</v>
-      </c>
-      <c r="I11" s="18">
         <v>0.9</v>
       </c>
-      <c r="J11" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I11" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="1">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="B12" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D12" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C12" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>13</v>
-      </c>
       <c r="E12" s="3">
         <v>1</v>
       </c>
       <c r="F12" s="4">
-        <v>45072</v>
+        <v>45073</v>
       </c>
       <c r="G12" s="4">
         <v>45075</v>
       </c>
       <c r="H12" s="2"/>
       <c r="I12" s="2"/>
-      <c r="J12" s="2"/>
-    </row>
-    <row r="13" spans="1:10" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="13" spans="1:9" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="1">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B13" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D13" s="2" t="s">
         <v>17</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>18</v>
       </c>
       <c r="E13" s="3">
         <v>1</v>
@@ -1010,7 +979,6 @@
       </c>
       <c r="H13" s="2"/>
       <c r="I13" s="2"/>
-      <c r="J13" s="2"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1:J13">

</xml_diff>